<commit_message>
Update Template and Trays
remove "bold" feature in  line 2
</commit_message>
<xml_diff>
--- a/Data/DWA_Template.xlsx
+++ b/Data/DWA_Template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Envimaster\Digitalisierung2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Envimaster\DWA\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1130A11B-56A7-4F2C-A46A-FC83720B4168}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EB79EF3-0670-43E6-9C1D-DB51240569D1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -193,7 +193,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -220,13 +220,6 @@
       <b/>
       <i/>
       <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -272,11 +265,11 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Heading" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -598,7 +591,7 @@
   <dimension ref="A1:BB5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -615,7 +608,7 @@
     <col min="16" max="16" width="14.875" customWidth="1"/>
     <col min="17" max="19" width="18.25" customWidth="1"/>
     <col min="20" max="20" width="15.5" customWidth="1"/>
-    <col min="21" max="21" width="15.5" style="3" customWidth="1"/>
+    <col min="21" max="21" width="15.5" style="1" customWidth="1"/>
     <col min="22" max="22" width="15.5" customWidth="1"/>
     <col min="23" max="23" width="10.75" customWidth="1"/>
     <col min="24" max="24" width="17.125" customWidth="1"/>
@@ -624,180 +617,180 @@
     <col min="33" max="33" width="10.75" customWidth="1"/>
     <col min="34" max="34" width="21.25" customWidth="1"/>
     <col min="35" max="50" width="10.75" customWidth="1"/>
-    <col min="51" max="51" width="10.75" style="3" customWidth="1"/>
+    <col min="51" max="51" width="10.75" style="1" customWidth="1"/>
     <col min="52" max="52" width="10.75" customWidth="1"/>
-    <col min="53" max="53" width="19" style="3" customWidth="1"/>
+    <col min="53" max="53" width="19" style="1" customWidth="1"/>
     <col min="54" max="1023" width="10.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:54" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="R1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="S1" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="T1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="U1" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="V1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="W1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="X1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="Y1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="Z1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AA1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AB1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="AC1" s="4" t="s">
+      <c r="AC1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="AD1" s="4" t="s">
+      <c r="AD1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AE1" s="4" t="s">
+      <c r="AE1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AF1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AG1" s="4" t="s">
+      <c r="AG1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AH1" s="4" t="s">
+      <c r="AH1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AI1" s="4" t="s">
+      <c r="AI1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AJ1" s="4" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AK1" s="4" t="s">
+      <c r="AK1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AL1" s="4" t="s">
+      <c r="AL1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AM1" s="4" t="s">
+      <c r="AM1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="AN1" s="4" t="s">
+      <c r="AN1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AO1" s="4" t="s">
+      <c r="AO1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AP1" s="4" t="s">
+      <c r="AP1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="AQ1" s="4" t="s">
+      <c r="AQ1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="AR1" s="4" t="s">
+      <c r="AR1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AS1" s="4" t="s">
+      <c r="AS1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AT1" s="4" t="s">
+      <c r="AT1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AU1" s="4" t="s">
+      <c r="AU1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AV1" s="4" t="s">
+      <c r="AV1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="AW1" s="4" t="s">
+      <c r="AW1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="AX1" s="4" t="s">
+      <c r="AX1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AY1" s="5" t="s">
+      <c r="AY1" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="AZ1" s="4" t="s">
+      <c r="AZ1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="BA1" s="5" t="s">
+      <c r="BA1" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="BB1" s="4" t="s">
+      <c r="BB1" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:54" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="U2" s="2"/>
-      <c r="AY2" s="2"/>
-      <c r="BA2" s="2"/>
+    <row r="2" spans="1:54" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="U2" s="5"/>
+      <c r="AY2" s="5"/>
+      <c r="BA2" s="5"/>
     </row>
     <row r="5" spans="1:54" x14ac:dyDescent="0.2">
       <c r="AZ5" t="s">

</xml_diff>